<commit_message>
update database + erreur datetimes
</commit_message>
<xml_diff>
--- a/backend/reports/projet_a48c395b-20eb-43cd-bdec-a7170c26daf2.xlsx
+++ b/backend/reports/projet_a48c395b-20eb-43cd-bdec-a7170c26daf2.xlsx
@@ -528,12 +528,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>-17.18%</t>
+          <t>-17.24%</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>81.10%</t>
+          <t>42.81%</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -551,13 +551,13 @@
         <v>15960</v>
       </c>
       <c r="L2" t="n">
-        <v>41362.44202950156</v>
+        <v>21832.06633969315</v>
       </c>
       <c r="M2" t="n">
-        <v>41362.44202950156</v>
+        <v>21832.06633969315</v>
       </c>
       <c r="N2" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -725,34 +725,34 @@
         <v>8798</v>
       </c>
       <c r="E2" t="n">
-        <v>7487.920963602286</v>
+        <v>7518.764298007208</v>
       </c>
       <c r="F2" t="n">
         <v>8433.333333333332</v>
       </c>
       <c r="G2" t="n">
-        <v>-8759.254296935618</v>
+        <v>-8790.097631340541</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>-8759.254296935618</v>
+        <v>-8790.097631340541</v>
       </c>
       <c r="J2" t="n">
-        <v>-6037.033231594203</v>
+        <v>-4132.9656862278</v>
       </c>
       <c r="K2" t="n">
-        <v>7031.112267991917</v>
+        <v>5096.201388220592</v>
       </c>
       <c r="L2" t="n">
-        <v>-57037.03323159421</v>
+        <v>-55132.9656862278</v>
       </c>
       <c r="M2" t="n">
-        <v>-57037.03323159421</v>
+        <v>-55132.9656862278</v>
       </c>
       <c r="N2" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O2" t="n">
         <v>251000</v>
@@ -764,10 +764,10 @@
         <v>242566.6666666667</v>
       </c>
       <c r="R2" t="n">
-        <v>-7439.2542969356</v>
+        <v>-7470.097631340526</v>
       </c>
       <c r="S2" t="n">
-        <v>192968.887732008</v>
+        <v>194903.7986117794</v>
       </c>
       <c r="T2" t="n">
         <v>1800</v>
@@ -805,34 +805,34 @@
         <v>5913.959999999999</v>
       </c>
       <c r="E3" t="n">
-        <v>7237.84572440878</v>
+        <v>7337.507943029175</v>
       </c>
       <c r="F3" t="n">
         <v>8433.333333333332</v>
       </c>
       <c r="G3" t="n">
-        <v>-5305.939057742111</v>
+        <v>-5405.601276362506</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>-5305.939057742111</v>
+        <v>-5405.601276362506</v>
       </c>
       <c r="J3" t="n">
-        <v>-2807.393231594199</v>
+        <v>-903.3256862277967</v>
       </c>
       <c r="K3" t="n">
-        <v>7281.187507185422</v>
+        <v>5277.457743198624</v>
       </c>
       <c r="L3" t="n">
-        <v>-59844.42646318841</v>
+        <v>-56036.2913724556</v>
       </c>
       <c r="M3" t="n">
-        <v>-59844.42646318841</v>
+        <v>-56036.2913724556</v>
       </c>
       <c r="N3" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O3" t="n">
         <v>251000</v>
@@ -844,10 +844,10 @@
         <v>234133.3333333333</v>
       </c>
       <c r="R3" t="n">
-        <v>-11398.79335467765</v>
+        <v>-11529.29890770296</v>
       </c>
       <c r="S3" t="n">
-        <v>185687.7002248226</v>
+        <v>189626.3408685807</v>
       </c>
       <c r="T3" t="n">
         <v>1836</v>
@@ -885,34 +885,34 @@
         <v>6032.2392</v>
       </c>
       <c r="E4" t="n">
-        <v>6978.876070949928</v>
+        <v>7149.804851802482</v>
       </c>
       <c r="F4" t="n">
         <v>8433.333333333332</v>
       </c>
       <c r="G4" t="n">
-        <v>-4839.664604283261</v>
+        <v>-5010.593385135814</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>-4839.664604283261</v>
+        <v>-5010.593385135814</v>
       </c>
       <c r="J4" t="n">
-        <v>-2573.160431594201</v>
+        <v>-669.0928862277988</v>
       </c>
       <c r="K4" t="n">
-        <v>7540.157160644274</v>
+        <v>5465.160834425318</v>
       </c>
       <c r="L4" t="n">
-        <v>-62417.58689478261</v>
+        <v>-56705.3842586834</v>
       </c>
       <c r="M4" t="n">
-        <v>-62417.58689478261</v>
+        <v>-56705.3842586834</v>
       </c>
       <c r="N4" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O4" t="n">
         <v>251000</v>
@@ -924,10 +924,10 @@
         <v>225700</v>
       </c>
       <c r="R4" t="n">
-        <v>-14865.12995896096</v>
+        <v>-15166.5642928388</v>
       </c>
       <c r="S4" t="n">
-        <v>178147.5430641783</v>
+        <v>184161.1800341554</v>
       </c>
       <c r="T4" t="n">
         <v>1872.72</v>
@@ -965,34 +965,34 @@
         <v>6152.883984000002</v>
       </c>
       <c r="E5" t="n">
-        <v>6710.695656012073</v>
+        <v>6955.425733562317</v>
       </c>
       <c r="F5" t="n">
         <v>8433.333333333332</v>
       </c>
       <c r="G5" t="n">
-        <v>-4360.033293345406</v>
+        <v>-4604.763370895649</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>-4360.033293345406</v>
+        <v>-4604.763370895649</v>
       </c>
       <c r="J5" t="n">
-        <v>-2334.242975594204</v>
+        <v>-430.1754302278023</v>
       </c>
       <c r="K5" t="n">
-        <v>7808.337575582129</v>
+        <v>5659.539952665484</v>
       </c>
       <c r="L5" t="n">
-        <v>-64751.82987037682</v>
+        <v>-57135.55968891121</v>
       </c>
       <c r="M5" t="n">
-        <v>-64751.82987037682</v>
+        <v>-57135.55968891121</v>
       </c>
       <c r="N5" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O5" t="n">
         <v>251000</v>
@@ -1004,10 +1004,10 @@
         <v>217266.6666666667</v>
       </c>
       <c r="R5" t="n">
-        <v>-17824.36869230639</v>
+        <v>-18370.53310373443</v>
       </c>
       <c r="S5" t="n">
-        <v>170339.2054885963</v>
+        <v>178501.6400814899</v>
       </c>
       <c r="T5" t="n">
         <v>1910.1744</v>
@@ -1045,34 +1045,34 @@
         <v>6275.94166368</v>
       </c>
       <c r="E6" t="n">
-        <v>6432.976880875091</v>
+        <v>6754.133142370022</v>
       </c>
       <c r="F6" t="n">
         <v>8433.333333333332</v>
       </c>
       <c r="G6" t="n">
-        <v>-3866.634604288422</v>
+        <v>-4187.790865783353</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>-3866.634604288422</v>
+        <v>-4187.790865783353</v>
       </c>
       <c r="J6" t="n">
-        <v>-2090.547170474202</v>
+        <v>-186.4796251077996</v>
       </c>
       <c r="K6" t="n">
-        <v>8086.056350719112</v>
+        <v>5860.832543857778</v>
       </c>
       <c r="L6" t="n">
-        <v>-66842.37704085102</v>
+        <v>-57322.03931401901</v>
       </c>
       <c r="M6" t="n">
-        <v>-66842.37704085102</v>
+        <v>-57322.03931401901</v>
       </c>
       <c r="N6" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O6" t="n">
         <v>251000</v>
@@ -1084,10 +1084,10 @@
         <v>208833.3333333333</v>
       </c>
       <c r="R6" t="n">
-        <v>-20262.19284539481</v>
+        <v>-21129.51351831775</v>
       </c>
       <c r="S6" t="n">
-        <v>162253.1491378771</v>
+        <v>172640.8075376321</v>
       </c>
       <c r="T6" t="n">
         <v>1948.377888</v>
@@ -1125,34 +1125,34 @@
         <v>6401.460496953601</v>
       </c>
       <c r="E7" t="n">
-        <v>6145.380495130598</v>
+        <v>6545.68118705842</v>
       </c>
       <c r="F7" t="n">
         <v>7433.333333333333</v>
       </c>
       <c r="G7" t="n">
-        <v>-2359.044706345534</v>
+        <v>-2759.345398273355</v>
       </c>
       <c r="H7" t="n">
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>-2359.044706345534</v>
+        <v>-2759.345398273355</v>
       </c>
       <c r="J7" t="n">
-        <v>-1841.977449251804</v>
+        <v>62.09009611459896</v>
       </c>
       <c r="K7" t="n">
-        <v>8373.652736463604</v>
+        <v>6069.28449916938</v>
       </c>
       <c r="L7" t="n">
-        <v>-68684.35449010282</v>
+        <v>-57259.94921790441</v>
       </c>
       <c r="M7" t="n">
-        <v>-68684.35449010282</v>
+        <v>-57259.94921790441</v>
       </c>
       <c r="N7" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O7" t="n">
         <v>251000</v>
@@ -1164,10 +1164,10 @@
         <v>201400</v>
       </c>
       <c r="R7" t="n">
-        <v>-21163.8508915164</v>
+        <v>-22431.47225636715</v>
       </c>
       <c r="S7" t="n">
-        <v>153879.4964014136</v>
+        <v>166571.5230384627</v>
       </c>
       <c r="T7" t="n">
         <v>1987.34544576</v>
@@ -1205,34 +1205,34 @@
         <v>6529.489706892673</v>
       </c>
       <c r="E8" t="n">
-        <v>5847.555182266901</v>
+        <v>6329.815230860754</v>
       </c>
       <c r="F8" t="n">
         <v>7433.333333333333</v>
       </c>
       <c r="G8" t="n">
-        <v>-1836.826011039468</v>
+        <v>-2319.08605963332</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>-1836.826011039468</v>
+        <v>-2319.08605963332</v>
       </c>
       <c r="J8" t="n">
-        <v>-1588.436333604956</v>
+        <v>315.6312117614461</v>
       </c>
       <c r="K8" t="n">
-        <v>8671.478049327301</v>
+        <v>6285.150455367046</v>
       </c>
       <c r="L8" t="n">
-        <v>-70272.79082370778</v>
+        <v>-56944.31800614297</v>
       </c>
       <c r="M8" t="n">
-        <v>-70272.79082370778</v>
+        <v>-56944.31800614297</v>
       </c>
       <c r="N8" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O8" t="n">
         <v>251000</v>
@@ -1244,10 +1244,10 @@
         <v>193966.6666666667</v>
       </c>
       <c r="R8" t="n">
-        <v>-21514.14250912737</v>
+        <v>-23264.02392257194</v>
       </c>
       <c r="S8" t="n">
-        <v>145208.0183520863</v>
+        <v>160286.3725830957</v>
       </c>
       <c r="T8" t="n">
         <v>2027.0923546752</v>
@@ -1285,34 +1285,34 @@
         <v>6660.079501030526</v>
       </c>
       <c r="E9" t="n">
-        <v>5539.137130514461</v>
+        <v>6106.271580356368</v>
       </c>
       <c r="F9" t="n">
         <v>7433.333333333333</v>
       </c>
       <c r="G9" t="n">
-        <v>-1299.52670919581</v>
+        <v>-1866.661159037717</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>-1299.52670919581</v>
+        <v>-1866.661159037717</v>
       </c>
       <c r="J9" t="n">
-        <v>-1329.824395645169</v>
+        <v>574.2431497212337</v>
       </c>
       <c r="K9" t="n">
-        <v>8979.896101079741</v>
+        <v>6508.694105871432</v>
       </c>
       <c r="L9" t="n">
-        <v>-71602.61521935294</v>
+        <v>-56370.07485642174</v>
       </c>
       <c r="M9" t="n">
-        <v>-71602.61521935294</v>
+        <v>-56370.07485642174</v>
       </c>
       <c r="N9" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O9" t="n">
         <v>251000</v>
@@ -1324,10 +1324,10 @@
         <v>186533.3333333333</v>
       </c>
       <c r="R9" t="n">
-        <v>-21297.40413702614</v>
+        <v>-23614.42000031256</v>
       </c>
       <c r="S9" t="n">
-        <v>136228.1222510065</v>
+        <v>153777.6784772242</v>
       </c>
       <c r="T9" t="n">
         <v>2067.634201768704</v>
@@ -1365,34 +1365,34 @@
         <v>6793.281091051137</v>
       </c>
       <c r="E10" t="n">
-        <v>5219.749588427654</v>
+        <v>5874.777163353122</v>
       </c>
       <c r="F10" t="n">
         <v>7433.333333333333</v>
       </c>
       <c r="G10" t="n">
-        <v>-746.6802920159616</v>
+        <v>-1401.70786694143</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>-746.6802920159616</v>
+        <v>-1401.70786694143</v>
       </c>
       <c r="J10" t="n">
-        <v>-1066.040218926186</v>
+        <v>838.0273264402158</v>
       </c>
       <c r="K10" t="n">
-        <v>9299.283643166547</v>
+        <v>6740.188522874678</v>
       </c>
       <c r="L10" t="n">
-        <v>-72668.65543827912</v>
+        <v>-55532.04752998152</v>
       </c>
       <c r="M10" t="n">
-        <v>-72668.65543827912</v>
+        <v>-55532.04752998152</v>
       </c>
       <c r="N10" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O10" t="n">
         <v>251000</v>
@@ -1404,10 +1404,10 @@
         <v>179100</v>
       </c>
       <c r="R10" t="n">
-        <v>-20497.4940461191</v>
+        <v>-23469.53748433103</v>
       </c>
       <c r="S10" t="n">
-        <v>126928.83860784</v>
+        <v>147037.4899543495</v>
       </c>
       <c r="T10" t="n">
         <v>2108.986885804078</v>
@@ -1445,34 +1445,34 @@
         <v>24855.53524220682</v>
       </c>
       <c r="E11" t="n">
-        <v>4889.002404659917</v>
+        <v>5635.049195313069</v>
       </c>
       <c r="F11" t="n">
         <v>7433.333333333333</v>
       </c>
       <c r="G11" t="n">
-        <v>-18104.19358498799</v>
+        <v>-18850.24037564114</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>-18104.19358498799</v>
+        <v>-18850.24037564114</v>
       </c>
       <c r="J11" t="n">
-        <v>-18723.36888800749</v>
+        <v>-16819.30134264109</v>
       </c>
       <c r="K11" t="n">
-        <v>9630.030826934286</v>
+        <v>6979.916490914731</v>
       </c>
       <c r="L11" t="n">
-        <v>-91392.02432628661</v>
+        <v>-72351.34887262262</v>
       </c>
       <c r="M11" t="n">
-        <v>-91392.02432628661</v>
+        <v>-72351.34887262262</v>
       </c>
       <c r="N11" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O11" t="n">
         <v>251000</v>
@@ -1484,10 +1484,10 @@
         <v>171666.6666666667</v>
       </c>
       <c r="R11" t="n">
-        <v>-37024.16544052564</v>
+        <v>-40742.25566939072</v>
       </c>
       <c r="S11" t="n">
-        <v>117298.8077809057</v>
+        <v>140057.5734634348</v>
       </c>
       <c r="T11" t="n">
         <v>2151.16662352016</v>
@@ -1525,34 +1525,34 @@
         <v>7067.729647129602</v>
       </c>
       <c r="E12" t="n">
-        <v>4546.4915513701</v>
+        <v>5386.794833913901</v>
       </c>
       <c r="F12" t="n">
         <v>4833.333333333333</v>
       </c>
       <c r="G12" t="n">
-        <v>3007.596411283293</v>
+        <v>2167.293128739491</v>
       </c>
       <c r="H12" t="n">
-        <v>451.1394616924939</v>
+        <v>325.0939693109237</v>
       </c>
       <c r="I12" t="n">
-        <v>2556.456949590799</v>
+        <v>1842.199159428568</v>
       </c>
       <c r="J12" t="n">
-        <v>-973.6787629068897</v>
+        <v>1056.434274841083</v>
       </c>
       <c r="K12" t="n">
-        <v>9972.541680224102</v>
+        <v>7228.170852313899</v>
       </c>
       <c r="L12" t="n">
-        <v>-92365.7030891935</v>
+        <v>-71294.91459778154</v>
       </c>
       <c r="M12" t="n">
-        <v>-92365.7030891935</v>
+        <v>-71294.91459778154</v>
       </c>
       <c r="N12" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O12" t="n">
         <v>251000</v>
@@ -1564,10 +1564,10 @@
         <v>166833.3333333333</v>
       </c>
       <c r="R12" t="n">
-        <v>-32858.63585654176</v>
+        <v>-37290.98387556906</v>
       </c>
       <c r="S12" t="n">
-        <v>107326.2661006816</v>
+        <v>132829.4026111209</v>
       </c>
       <c r="T12" t="n">
         <v>2194.189955990563</v>
@@ -1605,34 +1605,34 @@
         <v>7209.084240072194</v>
       </c>
       <c r="E13" t="n">
-        <v>4191.79863067784</v>
+        <v>5129.710821324217</v>
       </c>
       <c r="F13" t="n">
         <v>4833.333333333333</v>
       </c>
       <c r="G13" t="n">
-        <v>3610.037757895288</v>
+        <v>2672.125567248911</v>
       </c>
       <c r="H13" t="n">
-        <v>541.5056636842932</v>
+        <v>400.8188350873366</v>
       </c>
       <c r="I13" t="n">
-        <v>3068.532094210994</v>
+        <v>2271.306732161574</v>
       </c>
       <c r="J13" t="n">
-        <v>-784.115086291093</v>
+        <v>1260.639287672267</v>
       </c>
       <c r="K13" t="n">
-        <v>10327.23460091636</v>
+        <v>7485.254864903583</v>
       </c>
       <c r="L13" t="n">
-        <v>-93149.81817548459</v>
+        <v>-70034.27531010927</v>
       </c>
       <c r="M13" t="n">
-        <v>-93149.81817548459</v>
+        <v>-70034.27531010927</v>
       </c>
       <c r="N13" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O13" t="n">
         <v>251000</v>
@@ -1644,10 +1644,10 @@
         <v>162000</v>
       </c>
       <c r="R13" t="n">
-        <v>-28148.84967524985</v>
+        <v>-33378.42305632654</v>
       </c>
       <c r="S13" t="n">
-        <v>96999.03149976526</v>
+        <v>125344.1477462173</v>
       </c>
       <c r="T13" t="n">
         <v>2238.073755110374</v>
@@ -1685,34 +1685,34 @@
         <v>7353.265924873639</v>
       </c>
       <c r="E14" t="n">
-        <v>3824.49036356505</v>
+        <v>4863.483113755594</v>
       </c>
       <c r="F14" t="n">
         <v>4833.333333333333</v>
       </c>
       <c r="G14" t="n">
-        <v>4230.049419446204</v>
+        <v>3191.056669255661</v>
       </c>
       <c r="H14" t="n">
-        <v>634.5074129169307</v>
+        <v>478.6585003883492</v>
       </c>
       <c r="I14" t="n">
-        <v>3595.542006529274</v>
+        <v>2712.398168867312</v>
       </c>
       <c r="J14" t="n">
-        <v>-591.5883593439821</v>
+        <v>1468.328098551001</v>
       </c>
       <c r="K14" t="n">
-        <v>10694.54286802915</v>
+        <v>7751.482572472206</v>
       </c>
       <c r="L14" t="n">
-        <v>-93741.40653482857</v>
+        <v>-68565.94721155826</v>
       </c>
       <c r="M14" t="n">
-        <v>-93741.40653482857</v>
+        <v>-68565.94721155826</v>
       </c>
       <c r="N14" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O14" t="n">
         <v>251000</v>
@@ -1724,10 +1724,10 @@
         <v>157166.6666666667</v>
       </c>
       <c r="R14" t="n">
-        <v>-22879.228499898</v>
+        <v>-28991.94571863663</v>
       </c>
       <c r="S14" t="n">
-        <v>86304.48863173612</v>
+        <v>117592.6651737451</v>
       </c>
       <c r="T14" t="n">
         <v>2282.835230212582</v>
@@ -1765,34 +1765,34 @@
         <v>7500.331243371113</v>
       </c>
       <c r="E15" t="n">
-        <v>3444.118060599194</v>
+        <v>4587.786497838964</v>
       </c>
       <c r="F15" t="n">
         <v>4833.333333333333</v>
       </c>
       <c r="G15" t="n">
-        <v>4868.17918473895</v>
+        <v>3724.51074749918</v>
       </c>
       <c r="H15" t="n">
-        <v>730.2268777108426</v>
+        <v>558.676612124877</v>
       </c>
       <c r="I15" t="n">
-        <v>4137.952307028107</v>
+        <v>3165.834135374303</v>
       </c>
       <c r="J15" t="n">
-        <v>-396.0687784345579</v>
+        <v>1679.549032517811</v>
       </c>
       <c r="K15" t="n">
-        <v>11074.91517099501</v>
+        <v>8027.179188388835</v>
       </c>
       <c r="L15" t="n">
-        <v>-94137.47531326313</v>
+        <v>-66886.39817904045</v>
       </c>
       <c r="M15" t="n">
-        <v>-94137.47531326313</v>
+        <v>-66886.39817904045</v>
       </c>
       <c r="N15" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O15" t="n">
         <v>251000</v>
@@ -1804,10 +1804,10 @@
         <v>152333.3333333334</v>
       </c>
       <c r="R15" t="n">
-        <v>-17033.71544067084</v>
+        <v>-24118.55083106329</v>
       </c>
       <c r="S15" t="n">
-        <v>75229.57346074109</v>
+        <v>109565.4859853562</v>
       </c>
       <c r="T15" t="n">
         <v>2328.491934816834</v>
@@ -1845,34 +1845,34 @@
         <v>7650.337868238536</v>
       </c>
       <c r="E16" t="n">
-        <v>3050.217073831799</v>
+        <v>4302.284193356665</v>
       </c>
       <c r="F16" t="n">
         <v>4833.333333333333</v>
       </c>
       <c r="G16" t="n">
-        <v>5524.992783079775</v>
+        <v>4272.925663554908</v>
       </c>
       <c r="H16" t="n">
-        <v>828.7489174619662</v>
+        <v>640.9388495332362</v>
       </c>
       <c r="I16" t="n">
-        <v>4696.243865617809</v>
+        <v>3631.986814021672</v>
       </c>
       <c r="J16" t="n">
-        <v>-197.5269915682696</v>
+        <v>1894.350621726863</v>
       </c>
       <c r="K16" t="n">
-        <v>11468.8161577624</v>
+        <v>8312.681492871134</v>
       </c>
       <c r="L16" t="n">
-        <v>-94335.0023048314</v>
+        <v>-64992.04755731358</v>
       </c>
       <c r="M16" t="n">
-        <v>-94335.0023048314</v>
+        <v>-64992.04755731358</v>
       </c>
       <c r="N16" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O16" t="n">
         <v>251000</v>
@@ -1884,10 +1884,10 @@
         <v>147500</v>
       </c>
       <c r="R16" t="n">
-        <v>-10595.75960781006</v>
+        <v>-18744.85204979863</v>
       </c>
       <c r="S16" t="n">
-        <v>63760.75730297869</v>
+        <v>101252.8044924851</v>
       </c>
       <c r="T16" t="n">
         <v>2375.06177351317</v>
@@ -1925,34 +1925,34 @@
         <v>7803.344625603305</v>
       </c>
       <c r="E17" t="n">
-        <v>2642.306229202678</v>
+        <v>4006.627441844878</v>
       </c>
       <c r="F17" t="n">
         <v>3500</v>
       </c>
       <c r="G17" t="n">
-        <v>7534.40782484713</v>
+        <v>6170.086612204929</v>
       </c>
       <c r="H17" t="n">
-        <v>1130.161173727069</v>
+        <v>925.5129918307393</v>
       </c>
       <c r="I17" t="n">
-        <v>6404.24665112006</v>
+        <v>5244.57362037419</v>
       </c>
       <c r="J17" t="n">
-        <v>-195.9341446836104</v>
+        <v>1912.781582579122</v>
       </c>
       <c r="K17" t="n">
-        <v>11876.72700239152</v>
+        <v>8608.338244382921</v>
       </c>
       <c r="L17" t="n">
-        <v>-94530.93644951501</v>
+        <v>-63079.26597473446</v>
       </c>
       <c r="M17" t="n">
-        <v>-94530.93644951501</v>
+        <v>-63079.26597473446</v>
       </c>
       <c r="N17" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O17" t="n">
         <v>251000</v>
@@ -1964,10 +1964,10 @@
         <v>144000</v>
       </c>
       <c r="R17" t="n">
-        <v>-2414.966750102147</v>
+        <v>-11723.7322228366</v>
       </c>
       <c r="S17" t="n">
-        <v>51884.03030058717</v>
+        <v>92644.46624810217</v>
       </c>
       <c r="T17" t="n">
         <v>2422.563008983434</v>
@@ -2005,34 +2005,34 @@
         <v>7959.411518115372</v>
       </c>
       <c r="E18" t="n">
-        <v>2219.887238756482</v>
+        <v>3700.455080563913</v>
       </c>
       <c r="F18" t="n">
         <v>3500</v>
       </c>
       <c r="G18" t="n">
-        <v>8230.361096374323</v>
+        <v>6749.793254566891</v>
       </c>
       <c r="H18" t="n">
-        <v>1234.554164456148</v>
+        <v>1012.468988185034</v>
       </c>
       <c r="I18" t="n">
-        <v>6995.806931918175</v>
+        <v>5737.324266381857</v>
       </c>
       <c r="J18" t="n">
-        <v>8.738069800062249</v>
+        <v>2134.89079143758</v>
       </c>
       <c r="K18" t="n">
-        <v>12299.14599283772</v>
+        <v>8914.510605663887</v>
       </c>
       <c r="L18" t="n">
-        <v>-94522.19837971494</v>
+        <v>-60944.37518329688</v>
       </c>
       <c r="M18" t="n">
-        <v>-94522.19837971494</v>
+        <v>-60944.37518329688</v>
       </c>
       <c r="N18" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O18" t="n">
         <v>251000</v>
@@ -2044,10 +2044,10 @@
         <v>140500</v>
       </c>
       <c r="R18" t="n">
-        <v>6392.917312535639</v>
+        <v>-4174.330825735131</v>
       </c>
       <c r="S18" t="n">
-        <v>39584.88430774945</v>
+        <v>83729.95564243828</v>
       </c>
       <c r="T18" t="n">
         <v>2471.014269163103</v>
@@ -2085,34 +2085,34 @@
         <v>8118.599748477679</v>
       </c>
       <c r="E19" t="n">
-        <v>1782.444091953601</v>
+        <v>3383.39310131591</v>
       </c>
       <c r="F19" t="n">
         <v>3500</v>
       </c>
       <c r="G19" t="n">
-        <v>8946.809209879821</v>
+        <v>7345.860200517511</v>
       </c>
       <c r="H19" t="n">
-        <v>1342.021381481973</v>
+        <v>1101.879030077627</v>
       </c>
       <c r="I19" t="n">
-        <v>7604.787828397848</v>
+        <v>6243.981170439884</v>
       </c>
       <c r="J19" t="n">
-        <v>216.5173620912478</v>
+        <v>2360.727258861995</v>
       </c>
       <c r="K19" t="n">
-        <v>12736.5891396406</v>
+        <v>9231.57258491189</v>
       </c>
       <c r="L19" t="n">
-        <v>-94305.68101762369</v>
+        <v>-58583.64792443488</v>
       </c>
       <c r="M19" t="n">
-        <v>-94305.68101762369</v>
+        <v>-58583.64792443488</v>
       </c>
       <c r="N19" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O19" t="n">
         <v>251000</v>
@@ -2124,10 +2124,10 @@
         <v>137000</v>
       </c>
       <c r="R19" t="n">
-        <v>15846.02381426749</v>
+        <v>3917.96901803877</v>
       </c>
       <c r="S19" t="n">
-        <v>26848.29516810885</v>
+        <v>74498.38305752637</v>
       </c>
       <c r="T19" t="n">
         <v>2520.434554546365</v>
@@ -2165,34 +2165,34 @@
         <v>8280.971743447233</v>
       </c>
       <c r="E20" t="n">
-        <v>1329.442425331845</v>
+        <v>3055.054193571038</v>
       </c>
       <c r="F20" t="n">
         <v>3500</v>
       </c>
       <c r="G20" t="n">
-        <v>9684.395942538244</v>
+        <v>7958.784174299051</v>
       </c>
       <c r="H20" t="n">
-        <v>1452.659391380736</v>
+        <v>1193.817626144858</v>
       </c>
       <c r="I20" t="n">
-        <v>8231.736551157508</v>
+        <v>6764.966548154193</v>
       </c>
       <c r="J20" t="n">
-        <v>427.4307916958305</v>
+        <v>2590.340102298112</v>
       </c>
       <c r="K20" t="n">
-        <v>13189.59080626236</v>
+        <v>9559.911492656762</v>
       </c>
       <c r="L20" t="n">
-        <v>-93878.25022592786</v>
+        <v>-55993.30782213677</v>
       </c>
       <c r="M20" t="n">
-        <v>-93878.25022592786</v>
+        <v>-55993.30782213677</v>
       </c>
       <c r="N20" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O20" t="n">
         <v>251000</v>
@@ -2204,10 +2204,10 @@
         <v>133500</v>
       </c>
       <c r="R20" t="n">
-        <v>25963.04541222569</v>
+        <v>12568.22061299366</v>
       </c>
       <c r="S20" t="n">
-        <v>13658.70436184648</v>
+        <v>64938.47156486961</v>
       </c>
       <c r="T20" t="n">
         <v>2570.843245637292</v>
@@ -2245,34 +2245,34 @@
         <v>37582.81462887215</v>
       </c>
       <c r="E21" t="n">
-        <v>860.3288697489066</v>
+        <v>2715.037271344072</v>
       </c>
       <c r="F21" t="n">
         <v>3500</v>
       </c>
       <c r="G21" t="n">
-        <v>-18692.43718507739</v>
+        <v>-20547.14558667256</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>-18692.43718507739</v>
+        <v>-20547.14558667256</v>
       </c>
       <c r="J21" t="n">
-        <v>-26928.15079918599</v>
+        <v>-25024.08325381959</v>
       </c>
       <c r="K21" t="n">
-        <v>13658.7043618453</v>
+        <v>9899.928414883727</v>
       </c>
       <c r="L21" t="n">
-        <v>-120806.4010251139</v>
+        <v>-81017.39107595636</v>
       </c>
       <c r="M21" t="n">
-        <v>-120806.4010251139</v>
+        <v>-81017.39107595636</v>
       </c>
       <c r="N21" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O21" t="n">
         <v>251000</v>
@@ -2284,10 +2284,10 @@
         <v>130000</v>
       </c>
       <c r="R21" t="n">
-        <v>9193.598974884986</v>
+        <v>-6055.934225942219</v>
       </c>
       <c r="S21" t="n">
-        <v>1.189164322568104e-09</v>
+        <v>55038.54314998589</v>
       </c>
       <c r="T21" t="n">
         <v>2622.260110550038</v>
@@ -2325,34 +2325,34 @@
         <v>8615.523001882502</v>
       </c>
       <c r="E22" t="n">
-        <v>600</v>
+        <v>2362.926983243427</v>
       </c>
       <c r="F22" t="n">
         <v>3500</v>
       </c>
       <c r="G22" t="n">
-        <v>11000.19743793204</v>
+        <v>9237.270454688616</v>
       </c>
       <c r="H22" t="n">
-        <v>1650.029615689806</v>
+        <v>1385.590568203292</v>
       </c>
       <c r="I22" t="n">
-        <v>9350.167822242236</v>
+        <v>7851.679886485324</v>
       </c>
       <c r="J22" t="n">
-        <v>14811.61838493366</v>
+        <v>3061.091746192379</v>
       </c>
       <c r="K22" t="n">
-        <v>0</v>
+        <v>10252.03870298437</v>
       </c>
       <c r="L22" t="n">
-        <v>-105994.7826401802</v>
+        <v>-77956.29932976398</v>
       </c>
       <c r="M22" t="n">
-        <v>-105994.7826401802</v>
+        <v>-77956.29932976398</v>
       </c>
       <c r="N22" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O22" t="n">
         <v>251000</v>
@@ -2364,10 +2364,10 @@
         <v>126500</v>
       </c>
       <c r="R22" t="n">
-        <v>20505.21735981865</v>
+        <v>3757.19622323454</v>
       </c>
       <c r="S22" t="n">
-        <v>1.189164322568104e-09</v>
+        <v>44786.50444700151</v>
       </c>
       <c r="T22" t="n">
         <v>2674.705312761039</v>
@@ -2405,34 +2405,34 @@
         <v>8787.833461920151</v>
       </c>
       <c r="E23" t="n">
-        <v>600</v>
+        <v>1998.293205094113</v>
       </c>
       <c r="F23" t="n">
         <v>3500</v>
       </c>
       <c r="G23" t="n">
-        <v>11302.20138669068</v>
+        <v>9903.908181596571</v>
       </c>
       <c r="H23" t="n">
-        <v>1695.330208003603</v>
+        <v>1485.586227239486</v>
       </c>
       <c r="I23" t="n">
-        <v>9606.871178687081</v>
+        <v>8418.321954357085</v>
       </c>
       <c r="J23" t="n">
-        <v>15107.55075263234</v>
+        <v>3302.329047168658</v>
       </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>10616.67248113369</v>
       </c>
       <c r="L23" t="n">
-        <v>-90887.23188754785</v>
+        <v>-74653.97028259531</v>
       </c>
       <c r="M23" t="n">
-        <v>-90887.23188754785</v>
+        <v>-74653.97028259531</v>
       </c>
       <c r="N23" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O23" t="n">
         <v>251000</v>
@@ -2444,10 +2444,10 @@
         <v>123000</v>
       </c>
       <c r="R23" t="n">
-        <v>32112.76811245099</v>
+        <v>14176.19775153689</v>
       </c>
       <c r="S23" t="n">
-        <v>1.189164322568104e-09</v>
+        <v>34169.83196586783</v>
       </c>
       <c r="T23" t="n">
         <v>2728.19941901626</v>
@@ -2485,34 +2485,34 @@
         <v>8963.590131158555</v>
       </c>
       <c r="E24" t="n">
-        <v>600</v>
+        <v>1620.690514514852</v>
       </c>
       <c r="F24" t="n">
         <v>3500</v>
       </c>
       <c r="G24" t="n">
-        <v>11610.24541442449</v>
+        <v>10589.55489990964</v>
       </c>
       <c r="H24" t="n">
-        <v>1741.536812163674</v>
+        <v>1588.433234986446</v>
       </c>
       <c r="I24" t="n">
-        <v>9868.70860226082</v>
+        <v>9001.121664923196</v>
       </c>
       <c r="J24" t="n">
-        <v>15409.40176768498</v>
+        <v>3547.539658634411</v>
       </c>
       <c r="K24" t="n">
-        <v>0</v>
+        <v>10994.27517171295</v>
       </c>
       <c r="L24" t="n">
-        <v>-75477.83011986286</v>
+        <v>-71106.4306239609</v>
       </c>
       <c r="M24" t="n">
-        <v>-75477.83011986286</v>
+        <v>-71106.4306239609</v>
       </c>
       <c r="N24" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O24" t="n">
         <v>251000</v>
@@ -2524,10 +2524,10 @@
         <v>119500</v>
       </c>
       <c r="R24" t="n">
-        <v>44022.16988013598</v>
+        <v>25218.01258188425</v>
       </c>
       <c r="S24" t="n">
-        <v>1.189164322568104e-09</v>
+        <v>23175.55679415488</v>
       </c>
       <c r="T24" t="n">
         <v>2782.763407396585</v>
@@ -2565,34 +2565,34 @@
         <v>9142.861933781725</v>
       </c>
       <c r="E25" t="n">
-        <v>600</v>
+        <v>1229.657646807486</v>
       </c>
       <c r="F25" t="n">
         <v>3500</v>
       </c>
       <c r="G25" t="n">
-        <v>11924.45032271299</v>
+        <v>11294.7926759055</v>
       </c>
       <c r="H25" t="n">
-        <v>1788.667548406949</v>
+        <v>1694.218901385826</v>
       </c>
       <c r="I25" t="n">
-        <v>10135.78277430604</v>
+        <v>9600.573774519678</v>
       </c>
       <c r="J25" t="n">
-        <v>15717.28980303869</v>
+        <v>3796.772763832011</v>
       </c>
       <c r="K25" t="n">
-        <v>0</v>
+        <v>11385.30803942031</v>
       </c>
       <c r="L25" t="n">
-        <v>-59760.54031682418</v>
+        <v>-67309.65786012889</v>
       </c>
       <c r="M25" t="n">
-        <v>-59760.54031682418</v>
+        <v>-67309.65786012889</v>
       </c>
       <c r="N25" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O25" t="n">
         <v>251000</v>
@@ -2604,10 +2604,10 @@
         <v>116000</v>
       </c>
       <c r="R25" t="n">
-        <v>56239.45968317467</v>
+        <v>36900.09338513657</v>
       </c>
       <c r="S25" t="n">
-        <v>1.189164322568104e-09</v>
+        <v>11790.24875473456</v>
       </c>
       <c r="T25" t="n">
         <v>2838.418675544517</v>
@@ -2645,34 +2645,34 @@
         <v>9325.719172457362</v>
       </c>
       <c r="E26" t="n">
-        <v>600</v>
+        <v>824.7169314940439</v>
       </c>
       <c r="F26" t="n">
         <v>3500</v>
       </c>
       <c r="G26" t="n">
-        <v>12244.93932916725</v>
+        <v>12020.2223976732</v>
       </c>
       <c r="H26" t="n">
-        <v>1836.740899375087</v>
+        <v>1803.033359650981</v>
       </c>
       <c r="I26" t="n">
-        <v>10408.19842979216</v>
+        <v>10217.18903802222</v>
       </c>
       <c r="J26" t="n">
-        <v>16031.33559909946</v>
+        <v>4050.077452595768</v>
       </c>
       <c r="K26" t="n">
-        <v>0</v>
+        <v>11790.24875473376</v>
       </c>
       <c r="L26" t="n">
-        <v>-43729.20471772472</v>
+        <v>-63259.58040753313</v>
       </c>
       <c r="M26" t="n">
-        <v>-43729.20471772472</v>
+        <v>-63259.58040753313</v>
       </c>
       <c r="N26" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O26" t="n">
         <v>251000</v>
@@ -2684,10 +2684,10 @@
         <v>112500</v>
       </c>
       <c r="R26" t="n">
-        <v>68770.79528227412</v>
+        <v>49240.4195924661</v>
       </c>
       <c r="S26" t="n">
-        <v>1.189164322568104e-09</v>
+        <v>8.067218004725873e-10</v>
       </c>
       <c r="T26" t="n">
         <v>2895.187049055407</v>
@@ -2746,13 +2746,13 @@
         <v>0</v>
       </c>
       <c r="L27" t="n">
-        <v>-27377.54240664327</v>
+        <v>-46907.91809645168</v>
       </c>
       <c r="M27" t="n">
-        <v>-27377.54240664327</v>
+        <v>-46907.91809645168</v>
       </c>
       <c r="N27" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O27" t="n">
         <v>251000</v>
@@ -2764,10 +2764,10 @@
         <v>109000</v>
       </c>
       <c r="R27" t="n">
-        <v>81622.45759335556</v>
+        <v>62092.08190354754</v>
       </c>
       <c r="S27" t="n">
-        <v>1.189164322568104e-09</v>
+        <v>8.067218004725873e-10</v>
       </c>
       <c r="T27" t="n">
         <v>2953.090790036515</v>
@@ -2826,13 +2826,13 @@
         <v>0</v>
       </c>
       <c r="L28" t="n">
-        <v>-10699.14684934019</v>
+        <v>-30229.5225391486</v>
       </c>
       <c r="M28" t="n">
-        <v>-10699.14684934019</v>
+        <v>-30229.5225391486</v>
       </c>
       <c r="N28" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O28" t="n">
         <v>251000</v>
@@ -2844,10 +2844,10 @@
         <v>105500</v>
       </c>
       <c r="R28" t="n">
-        <v>94800.85315065864</v>
+        <v>75270.47746085063</v>
       </c>
       <c r="S28" t="n">
-        <v>1.189164322568104e-09</v>
+        <v>8.067218004725873e-10</v>
       </c>
       <c r="T28" t="n">
         <v>3012.152605837246</v>
@@ -2906,13 +2906,13 @@
         <v>0</v>
       </c>
       <c r="L29" t="n">
-        <v>6312.516619108952</v>
+        <v>-13217.85907069946</v>
       </c>
       <c r="M29" t="n">
-        <v>6312.516619108952</v>
+        <v>-13217.85907069946</v>
       </c>
       <c r="N29" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O29" t="n">
         <v>251000</v>
@@ -2924,10 +2924,10 @@
         <v>102000</v>
       </c>
       <c r="R29" t="n">
-        <v>108312.5166191078</v>
+        <v>88782.14092929977</v>
       </c>
       <c r="S29" t="n">
-        <v>1.189164322568104e-09</v>
+        <v>8.067218004725873e-10</v>
       </c>
       <c r="T29" t="n">
         <v>3072.39565795399</v>
@@ -2986,13 +2986,13 @@
         <v>0</v>
       </c>
       <c r="L30" t="n">
-        <v>23664.11335692708</v>
+        <v>4133.737667118665</v>
       </c>
       <c r="M30" t="n">
-        <v>23664.11335692708</v>
+        <v>4133.737667118665</v>
       </c>
       <c r="N30" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O30" t="n">
         <v>251000</v>
@@ -3004,10 +3004,10 @@
         <v>98500.00000000003</v>
       </c>
       <c r="R30" t="n">
-        <v>122164.1133569259</v>
+        <v>102633.7376671179</v>
       </c>
       <c r="S30" t="n">
-        <v>1.189164322568104e-09</v>
+        <v>8.067218004725873e-10</v>
       </c>
       <c r="T30" t="n">
         <v>3133.843571113071</v>
@@ -3066,13 +3066,13 @@
         <v>0</v>
       </c>
       <c r="L31" t="n">
-        <v>41362.44202950156</v>
+        <v>21832.06633969315</v>
       </c>
       <c r="M31" t="n">
-        <v>41362.44202950156</v>
+        <v>21832.06633969315</v>
       </c>
       <c r="N31" t="n">
-        <v>13919.0332315942</v>
+        <v>12014.9656862278</v>
       </c>
       <c r="O31" t="n">
         <v>251000</v>
@@ -3084,10 +3084,10 @@
         <v>95000.00000000003</v>
       </c>
       <c r="R31" t="n">
-        <v>136362.4420295004</v>
+        <v>116832.0663396924</v>
       </c>
       <c r="S31" t="n">
-        <v>1.189164322568104e-09</v>
+        <v>8.067218004725873e-10</v>
       </c>
       <c r="T31" t="n">
         <v>3196.520442535332</v>

</xml_diff>